<commit_message>
Aula 2 Python Finanças
</commit_message>
<xml_diff>
--- a/28 - Integração Python para Finanças/Carteira.xlsx
+++ b/28 - Integração Python para Finanças/Carteira.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaop\Google Drive\Python Impressionador\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thiarly/Desktop/PROJECTS/Impressionador-Python-Course/28 - Integração Python para Finanças/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D41AAFDD-6504-40ED-94D8-002E58556BE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8DE967F-38C7-DE40-9803-4378EBBE5BD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{DD22BB9C-EFA3-4458-A6C0-AD8BCF6ABA57}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23240" windowHeight="13160" xr2:uid="{DD22BB9C-EFA3-4458-A6C0-AD8BCF6ABA57}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
   <si>
     <t>Ativos</t>
   </si>
@@ -42,58 +42,55 @@
     <t>Qtde</t>
   </si>
   <si>
-    <t>BOVA11</t>
-  </si>
-  <si>
-    <t>SMAL11</t>
-  </si>
-  <si>
-    <t>MGLU3</t>
-  </si>
-  <si>
     <t>BBDC4</t>
   </si>
   <si>
-    <t>ITUB4</t>
-  </si>
-  <si>
-    <t>ENEV3</t>
-  </si>
-  <si>
-    <t>MOVI3</t>
-  </si>
-  <si>
-    <t>BPAC11</t>
-  </si>
-  <si>
     <t>GNDI3</t>
   </si>
   <si>
-    <t>BCRI11</t>
-  </si>
-  <si>
     <t>Tipo</t>
   </si>
   <si>
-    <t>ETF</t>
-  </si>
-  <si>
     <t>Ação</t>
   </si>
   <si>
     <t>FII</t>
   </si>
   <si>
-    <t>VILG11</t>
-  </si>
-  <si>
-    <t>KNRI11</t>
-  </si>
-  <si>
-    <t>NTCO3</t>
-  </si>
-  <si>
-    <t>XPLG11</t>
+    <t>BBDC3</t>
+  </si>
+  <si>
+    <t>BBAS3</t>
+  </si>
+  <si>
+    <t>JHSF3</t>
+  </si>
+  <si>
+    <t>EGIE3</t>
+  </si>
+  <si>
+    <t>ITSA4</t>
+  </si>
+  <si>
+    <t>ABCB4</t>
+  </si>
+  <si>
+    <t>TRPL4</t>
+  </si>
+  <si>
+    <t>RECR11</t>
+  </si>
+  <si>
+    <t>BBSE3</t>
+  </si>
+  <si>
+    <t>PASS3</t>
+  </si>
+  <si>
+    <t>FLRY3</t>
+  </si>
+  <si>
+    <t>WEGE3</t>
   </si>
 </sst>
 </file>
@@ -149,7 +146,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -447,170 +444,172 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D46BDEA6-15EF-4648-A84D-A167B09326D1}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C3">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <v>1000</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C5">
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C6">
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C7">
         <v>300</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C8">
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C9">
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C10">
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C11">
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C12">
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>16</v>
       </c>
       <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>15</v>
       </c>
-      <c r="C13">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" t="s">
-        <v>17</v>
-      </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C14">
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C15">
         <v>100</v>

</xml_diff>

<commit_message>
Aula 28, python para finanças
Estrutura de uma carteira nesse arquivo: Carteira de Ações com Excel.ipynb
</commit_message>
<xml_diff>
--- a/28 - Integração Python para Finanças/Carteira.xlsx
+++ b/28 - Integração Python para Finanças/Carteira.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thiarly/Desktop/PROJECTS/Impressionador-Python-Course/28 - Integração Python para Finanças/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8DE967F-38C7-DE40-9803-4378EBBE5BD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48DEFA8D-A3B1-7C46-B606-300B6D79EF4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23240" windowHeight="13160" xr2:uid="{DD22BB9C-EFA3-4458-A6C0-AD8BCF6ABA57}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
   <si>
     <t>Ativos</t>
   </si>
@@ -45,9 +45,6 @@
     <t>BBDC4</t>
   </si>
   <si>
-    <t>GNDI3</t>
-  </si>
-  <si>
     <t>Tipo</t>
   </si>
   <si>
@@ -84,13 +81,13 @@
     <t>BBSE3</t>
   </si>
   <si>
-    <t>PASS3</t>
-  </si>
-  <si>
     <t>FLRY3</t>
   </si>
   <si>
     <t>WEGE3</t>
+  </si>
+  <si>
+    <t>PSSA3</t>
   </si>
 </sst>
 </file>
@@ -442,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D46BDEA6-15EF-4648-A84D-A167B09326D1}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -455,7 +452,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -463,10 +460,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>100</v>
@@ -474,10 +471,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <v>100</v>
@@ -485,10 +482,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4">
         <v>1000</v>
@@ -499,7 +496,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5">
         <v>100</v>
@@ -507,10 +504,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6">
         <v>100</v>
@@ -518,10 +515,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7">
         <v>300</v>
@@ -529,10 +526,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8">
         <v>100</v>
@@ -540,10 +537,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C9">
         <v>100</v>
@@ -551,10 +548,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10">
         <v>100</v>
@@ -562,10 +559,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C11">
         <v>100</v>
@@ -576,7 +573,7 @@
         <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C12">
         <v>100</v>
@@ -584,10 +581,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C13">
         <v>100</v>
@@ -595,23 +592,12 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
       </c>
       <c r="C14">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15">
         <v>100</v>
       </c>
     </row>

</xml_diff>